<commit_message>
Weiß nicht ob die ips jetzt richtig sind und hab keine lust nachzusehen
</commit_message>
<xml_diff>
--- a/Challenge II/Services.xlsx
+++ b/Challenge II/Services.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tmarkmann\Documents\I-Tech\pb6\Challenge II\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05919F4B-49D6-40BB-956F-F46D0234AEC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3521EF-5EF9-41D9-B670-FD2ABC2C8249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -154,13 +154,13 @@
     <t>Tom Azure</t>
   </si>
   <si>
-    <t>20.107.94.83</t>
-  </si>
-  <si>
     <t>10.0.0.6/24</t>
   </si>
   <si>
     <t>20.8.110.60</t>
+  </si>
+  <si>
+    <t>108.143.141.90</t>
   </si>
 </sst>
 </file>
@@ -511,7 +511,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -519,7 +519,7 @@
     <col min="1" max="1" width="27.5546875" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="14.5546875" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" customWidth="1"/>
-    <col min="5" max="5" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="44.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="7" customWidth="1"/>
   </cols>
@@ -558,13 +558,13 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F2" t="s">
         <v>21</v>
@@ -581,13 +581,13 @@
         <v>15</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D3" t="s">
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G3" t="s">
         <v>31</v>
@@ -601,13 +601,13 @@
         <v>15</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>20</v>
@@ -630,7 +630,7 @@
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>22</v>
@@ -688,7 +688,7 @@
         <v>36</v>
       </c>
       <c r="E9" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
         <v>26</v>
@@ -705,13 +705,13 @@
         <v>15</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
         <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F10" t="s">
         <v>27</v>
@@ -728,13 +728,13 @@
         <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D11" t="s">
         <v>18</v>
       </c>
       <c r="E11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G11" t="s">
         <v>31</v>
@@ -751,13 +751,13 @@
         <v>15</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G12" t="s">
         <v>31</v>

</xml_diff>